<commit_message>
added cool excel sheets
</commit_message>
<xml_diff>
--- a/03_CONCEPTION_NOTES/power_tree.xlsx
+++ b/03_CONCEPTION_NOTES/power_tree.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School\Documents\S7_electronique_avance\03_CONCEPTION_NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F199D1-2BF0-4F10-A9F6-626365AA6E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60655B5F-02D5-4CB6-917F-F4C5B451943D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>IC</t>
   </si>
@@ -129,9 +140,6 @@
     <t>VBUS</t>
   </si>
   <si>
-    <t>5V</t>
-  </si>
-  <si>
     <t>MT41J128M16JT-125</t>
   </si>
   <si>
@@ -139,6 +147,84 @@
   </si>
   <si>
     <t>VDDQ</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>FPGA</t>
+  </si>
+  <si>
+    <t>JTAG_DEBUGGUER</t>
+  </si>
+  <si>
+    <t>USB CONN</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>TLP2362</t>
+  </si>
+  <si>
+    <t>Octoupleur</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>2.7 - 5.5V</t>
+  </si>
+  <si>
+    <t>ADUM3160BRWZ-RL</t>
+  </si>
+  <si>
+    <t>USB isolator</t>
+  </si>
+  <si>
+    <t>VDD2/VBUS2</t>
+  </si>
+  <si>
+    <t>VBUS1</t>
+  </si>
+  <si>
+    <t>PIN1</t>
+  </si>
+  <si>
+    <t>VDD1</t>
+  </si>
+  <si>
+    <t>VREF-UART</t>
+  </si>
+  <si>
+    <t>VREFDQ</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>VREFCA</t>
+  </si>
+  <si>
+    <t>590BD-BDG</t>
+  </si>
+  <si>
+    <t>xtal 125MHz</t>
+  </si>
+  <si>
+    <t>CDCE62005RGZT</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>VCC_IN_XX</t>
+  </si>
+  <si>
+    <t>PLL</t>
+  </si>
+  <si>
+    <t>VCC_OUT</t>
   </si>
 </sst>
 </file>
@@ -160,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +271,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -198,11 +296,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,10 +321,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3816014D-321F-4496-BB75-D9FE3B93155B}" name="Tableau1" displayName="Tableau1" ref="D3:AA7" totalsRowShown="0">
-  <autoFilter ref="D3:AA7" xr:uid="{3816014D-321F-4496-BB75-D9FE3B93155B}"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3816014D-321F-4496-BB75-D9FE3B93155B}" name="Tableau1" displayName="Tableau1" ref="C3:AA11" totalsRowShown="0">
+  <autoFilter ref="C3:AA11" xr:uid="{3816014D-321F-4496-BB75-D9FE3B93155B}"/>
+  <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{3250EFE0-D9A6-43E0-881A-1E2F65052EF9}" name="IC"/>
+    <tableColumn id="25" xr3:uid="{29AC5D4B-E30D-49EF-B245-55806969662D}" name="nickname"/>
     <tableColumn id="2" xr3:uid="{E4BEE50D-07FE-442F-94E1-A7A1183F8BAE}" name="Power Name 1"/>
     <tableColumn id="3" xr3:uid="{C752E68F-C1ED-4FED-A557-7240030ADB83}" name="Voltage 1"/>
     <tableColumn id="4" xr3:uid="{750801C3-DE36-463C-A59B-6E522275AF14}" name="Power Name 2"/>
@@ -516,38 +617,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AA7"/>
+  <dimension ref="A2:AA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" customWidth="1"/>
-    <col min="18" max="18" width="10.5546875" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" customWidth="1"/>
-    <col min="21" max="21" width="14.88671875" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" customWidth="1"/>
-    <col min="23" max="23" width="15.88671875" customWidth="1"/>
-    <col min="24" max="24" width="11.5546875" customWidth="1"/>
-    <col min="25" max="25" width="15.88671875" customWidth="1"/>
-    <col min="26" max="26" width="11.5546875" customWidth="1"/>
-    <col min="27" max="27" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+    <col min="20" max="20" width="14.88671875" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" customWidth="1"/>
+    <col min="22" max="22" width="14.88671875" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" customWidth="1"/>
+    <col min="24" max="24" width="15.88671875" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" customWidth="1"/>
+    <col min="26" max="26" width="15.88671875" customWidth="1"/>
+    <col min="27" max="27" width="11.5546875" customWidth="1"/>
+    <col min="28" max="28" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
@@ -559,8 +661,11 @@
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -636,13 +741,22 @@
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -656,33 +770,140 @@
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
+      <c r="F6" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
       <c r="F7">
         <v>1.5</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7">
         <v>1.5</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9">
+        <v>3.3</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11">
+        <v>3.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>